<commit_message>
fix and remove cn for tasks <=9 (jl check only view in mcp-tasks/final testset pool) [all use this index if not mentioned later]
</commit_message>
<xml_diff>
--- a/tasks/finalpool/excel-data-transformation/initial_workspace/Format_Example.xlsx
+++ b/tasks/finalpool/excel-data-transformation/initial_workspace/Format_Example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\zws_zju_Junior2\summer intern\MCP-Benchmark\excel_complex\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lockon\Desktop\tes\tmp\test\excel-data-transformation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F238207B-5E3D-4C67-8F98-233DCF36920D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08580E57-7945-4E98-BC0D-38C3185803A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Format_Example" sheetId="1" r:id="rId1"/>
@@ -22,12 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
   <si>
-    <t>2024-01</t>
-  </si>
-  <si>
-    <t>2024-02</t>
-  </si>
-  <si>
     <t>Time</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -36,14 +30,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Household Refrigerator</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Air Conditioner</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Household Washing Machines</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -62,12 +48,27 @@
   <si>
     <t>Accumulated Growth (%)</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024-12</t>
+  </si>
+  <si>
+    <t>Household Refrigerators</t>
+  </si>
+  <si>
+    <t>Air Conditioners</t>
+  </si>
+  <si>
+    <t>2024-11</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="0.0"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -117,7 +118,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -125,11 +126,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -430,162 +445,165 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.69140625" defaultRowHeight="14.15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.1796875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="30.08984375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="45.54296875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="44.36328125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="27.81640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="34.6328125" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="8.7265625" style="2"/>
+    <col min="1" max="1" width="10.15234375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="30.07421875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="45.53515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="44.3828125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="27.84375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="34.61328125" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="8.69140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2">
+        <v>899.1</v>
+      </c>
+      <c r="D2" s="2">
+        <v>10395.700000000001</v>
+      </c>
+      <c r="E2" s="3">
+        <v>10.299999999999999</v>
+      </c>
+      <c r="F2" s="3">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2369.5</v>
+      </c>
+      <c r="D3" s="2">
+        <v>26598.400000000001</v>
+      </c>
+      <c r="E3" s="3">
+        <v>12.9</v>
+      </c>
+      <c r="F3" s="3">
+        <v>9.6999999999999993</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="C4" s="2">
+        <v>1226.5</v>
+      </c>
+      <c r="D4" s="2">
+        <v>11736.5</v>
+      </c>
+      <c r="E4" s="3">
+        <v>27.900000000000002</v>
+      </c>
+      <c r="F4" s="3">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="C5" s="2">
+        <v>860.9</v>
+      </c>
+      <c r="D5" s="2">
+        <v>9588.5</v>
+      </c>
+      <c r="E5" s="3">
+        <v>2.6</v>
+      </c>
+      <c r="F5" s="3">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="C6" s="2">
+        <v>1967.9</v>
+      </c>
+      <c r="D6" s="2">
+        <v>24237.4</v>
+      </c>
+      <c r="E6" s="3">
+        <v>27</v>
+      </c>
+      <c r="F6" s="3">
+        <v>9.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2">
-        <v>245.6</v>
-      </c>
-      <c r="D2" s="2">
-        <v>245.6</v>
-      </c>
-      <c r="E2" s="2">
-        <v>5.2</v>
-      </c>
-      <c r="F2" s="2">
-        <v>5.2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2">
-        <v>892.3</v>
-      </c>
-      <c r="D3" s="2">
-        <v>892.3</v>
-      </c>
-      <c r="E3" s="2">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="F3" s="2">
-        <v>8.6999999999999993</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="2">
-        <v>456.8</v>
-      </c>
-      <c r="D4" s="2">
-        <v>456.8</v>
-      </c>
-      <c r="E4" s="2">
-        <v>3.9</v>
-      </c>
-      <c r="F4" s="2">
-        <v>3.9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="2">
-        <v>278.89999999999998</v>
-      </c>
-      <c r="D5" s="2">
-        <v>524.5</v>
-      </c>
-      <c r="E5" s="2">
-        <v>6.1</v>
-      </c>
-      <c r="F5" s="2">
-        <v>5.7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="2">
-        <v>756.4</v>
-      </c>
-      <c r="D6" s="2">
-        <v>1648.7</v>
-      </c>
-      <c r="E6" s="2">
-        <v>4.3</v>
-      </c>
-      <c r="F6" s="2">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="B7" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C7" s="2">
-        <v>512.1</v>
+        <v>1112.7</v>
       </c>
       <c r="D7" s="2">
-        <v>968.9</v>
-      </c>
-      <c r="E7" s="2">
-        <v>7.2</v>
-      </c>
-      <c r="F7" s="2">
-        <v>5.5</v>
+        <v>10458.200000000001</v>
+      </c>
+      <c r="E7" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="F7" s="3">
+        <v>6.3</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="B2:B4">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>